<commit_message>
Add Freetown dBootcamp to list of events
</commit_message>
<xml_diff>
--- a/past dBootcamp events.xlsx
+++ b/past dBootcamp events.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Serah\Documents\GitHub\dBootcamps\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26519"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="33600" windowHeight="21000"/>
   </bookViews>
   <sheets>
     <sheet name="past dBootcamp events" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="127">
   <si>
     <t>d|Bootcamp location</t>
   </si>
@@ -391,13 +391,22 @@
   </si>
   <si>
     <t>&gt;&gt;&gt;&gt;&gt;&gt;&gt; origin/master</t>
+  </si>
+  <si>
+    <t>Freetown, Sierra Leone</t>
+  </si>
+  <si>
+    <t>http://freetown.dbootcamp.org</t>
+  </si>
+  <si>
+    <t>June 14-17, 2016</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -532,6 +541,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -830,7 +855,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -873,13 +898,16 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -908,11 +936,13 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -979,7 +1009,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1014,7 +1044,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1191,7 +1221,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1199,15 +1229,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1224,7 +1258,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1241,7 +1275,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1258,7 +1292,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1275,7 +1309,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1292,7 +1326,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1309,7 +1343,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1326,7 +1360,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1343,7 +1377,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1360,7 +1394,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1377,7 +1411,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1394,7 +1428,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1411,7 +1445,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1428,7 +1462,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1445,7 +1479,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1462,7 +1496,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1479,7 +1513,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1496,7 +1530,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -1513,7 +1547,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1530,7 +1564,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -1547,7 +1581,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -1564,7 +1598,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -1581,7 +1615,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>65</v>
       </c>
@@ -1598,7 +1632,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -1615,7 +1649,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -1632,7 +1666,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -1649,7 +1683,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -1666,7 +1700,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>80</v>
       </c>
@@ -1683,7 +1717,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -1700,381 +1734,419 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30">
+        <v>8.4841460000000009</v>
+      </c>
+      <c r="C30">
+        <v>-13.2286</v>
+      </c>
+      <c r="D30" t="s">
+        <v>126</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
         <v>87</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>88</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>89</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
         <v>39</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
         <v>14</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
         <v>56</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>58</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>93</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
         <v>62</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
         <v>50</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
         <v>22</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
         <v>97</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>98</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D39" s="2">
         <v>42248</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
         <v>100</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>101</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D39">
+      <c r="D40">
         <v>2015</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
         <v>27</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
         <v>45</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
         <v>33</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
         <v>80</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>82</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
         <v>108</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>85</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
         <v>71</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>73</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
         <v>74</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>76</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
         <v>65</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>67</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
         <v>17</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>49</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
         <v>59</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>61</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
         <v>42</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
         <v>36</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>38</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D52" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
         <v>30</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>32</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D53" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
         <v>11</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>13</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
         <v>8</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>21</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
         <v>25</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>26</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>120</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D56" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
         <v>121</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>79</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>122</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D57" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>124</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D58" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
         <v>123</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B58" r:id="rId1"/>
+    <hyperlink ref="E30" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>